<commit_message>
added suport for waiting jquery to load
</commit_message>
<xml_diff>
--- a/Patrick/TestData/Sanity.xlsx
+++ b/Patrick/TestData/Sanity.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t xml:space="preserve">test 1 </t>
   </si>
@@ -40,9 +40,6 @@
     <t>funcA</t>
   </si>
   <si>
-    <t>funcB</t>
-  </si>
-  <si>
     <t>yoram</t>
   </si>
   <si>
@@ -131,6 +128,9 @@
   </si>
   <si>
     <t>TESTCASE</t>
+  </si>
+  <si>
+    <t>funcC</t>
   </si>
 </sst>
 </file>
@@ -475,7 +475,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -488,71 +488,71 @@
   <sheetData>
     <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>0</v>
@@ -561,66 +561,64 @@
         <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>

</xml_diff>